<commit_message>
Deployed 17d362a with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA/example_output/Taxonomic_assignments/CommonNames_required.xlsx
+++ b/eDNA/example_output/Taxonomic_assignments/CommonNames_required.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,24 +377,45 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cololabis saira</t>
+          <t>Fundulus heteroclitus or majalis</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Cololabis saira</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Unassigned</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Unassigned</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Unassigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mareca americana</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Myrophis vafer</t>
         </is>
       </c>
     </row>

</xml_diff>